<commit_message>
cart, pofile page, order track. admin panel baki
</commit_message>
<xml_diff>
--- a/Time_required.xlsx
+++ b/Time_required.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Aam-Niketon-Fronted\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFF04AD-F5E8-490C-B99D-137D9AAED311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33DE149-03EF-4C20-AC0C-70FCDA680C04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Serial No.</t>
   </si>
@@ -53,6 +53,15 @@
   </si>
   <si>
     <t>Home, Category, Product Details, Cart Pages Done</t>
+  </si>
+  <si>
+    <t>16-05-2022</t>
+  </si>
+  <si>
+    <t>2 hours 30 minutes</t>
+  </si>
+  <si>
+    <t>Log, Registration Page, Home page , project setup, add product and category funtionality implement</t>
   </si>
 </sst>
 </file>
@@ -443,7 +452,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,11 +508,21 @@
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
+      <c r="B3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.3125</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">

</xml_diff>